<commit_message>
Revised data files to make them R-friendly
</commit_message>
<xml_diff>
--- a/Data/quiz/e3v3/berlin_marathon.xlsx
+++ b/Data/quiz/e3v3/berlin_marathon.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kalarson\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\craigaj\Documents\GitHub\M221R\Data\quiz\e3v3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{138ADE5C-C759-4354-AC71-7BFA822C7CB0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8829EF1-DDFC-428B-8FE4-D7B49448B509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{310FA6AF-8FBB-4DE0-A8A4-78AD2877A4A1}"/>
   </bookViews>
@@ -33,10 +33,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>Female</t>
+    <t>female</t>
   </si>
   <si>
-    <t>Male</t>
+    <t>male</t>
   </si>
 </sst>
 </file>
@@ -390,9 +390,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A35834C0-2523-4372-82AE-E87415D73865}">
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>